<commit_message>
[Vinay] Modified the FinancialTransactions feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -101,7 +101,7 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -124,12 +124,6 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +172,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,10 +188,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,7 +196,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,72 +220,72 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="1" t="n">
         <v>944177</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -303,10 +297,10 @@
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -318,10 +312,10 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -333,10 +327,10 @@
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -348,10 +342,10 @@
       <c r="A7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="n">
@@ -360,13 +354,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="n">
@@ -378,10 +372,10 @@
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="6" t="n">
@@ -396,7 +390,7 @@
       <c r="B10" s="1" t="n">
         <v>944168</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="7" t="n">
@@ -411,7 +405,7 @@
       <c r="B11" s="1" t="n">
         <v>1245501</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="n">
@@ -419,14 +413,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>944162</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="n">

</xml_diff>

<commit_message>
[Vinay] Modified the FinancialTransactional Feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -89,17 +89,30 @@
   </si>
   <si>
     <t xml:space="preserve">accountsOfficer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assistantExaminer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0947241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0800129</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -167,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,6 +210,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,20 +238,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="24.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,10 +449,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" display="kurnool_eGov@123"/>
     <hyperlink ref="C12" r:id="rId2" display="kurnool_eGov@123"/>
+    <hyperlink ref="C13" r:id="rId3" display="kurnool_eGov@123"/>
+    <hyperlink ref="C14" r:id="rId4" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[Bimal] Created New Trade License Feature File
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -5,102 +5,100 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hasZone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juniorAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kurnool_eGov@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billCollector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">946800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0935528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egovernments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assistantEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0954568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seniorAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adm_manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assis_Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountsOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assistantExaminer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0947241</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examiner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0800129</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+  <si>
+    <t>dataName</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>hasZone</t>
+  </si>
+  <si>
+    <t>juniorAssistant</t>
+  </si>
+  <si>
+    <t>kurnool_eGov@123</t>
+  </si>
+  <si>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>0944206</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>944210</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>946800</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>0935528</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>egovernments</t>
+  </si>
+  <si>
+    <t>assistantEngineer</t>
+  </si>
+  <si>
+    <t>0954568</t>
+  </si>
+  <si>
+    <t>seniorAssistant</t>
+  </si>
+  <si>
+    <t>944186</t>
+  </si>
+  <si>
+    <t>adm_manager</t>
+  </si>
+  <si>
+    <t>assis_Engineer</t>
+  </si>
+  <si>
+    <t>accountsOfficer</t>
+  </si>
+  <si>
+    <t>assistantExaminer</t>
+  </si>
+  <si>
+    <t>0947241</t>
+  </si>
+  <si>
+    <t>examiner</t>
+  </si>
+  <si>
+    <t>0800129</t>
+  </si>
+  <si>
+    <t>creator</t>
   </si>
 </sst>
 </file>
@@ -108,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
@@ -180,27 +178,27 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,10 +212,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,75 +232,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="24.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3444444444444"/>
     <col collapsed="false" hidden="false" max="26" min="5" style="0" width="14.4037037037037"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="4" t="n">
         <v>944177</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -318,10 +312,10 @@
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -333,10 +327,10 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -348,10 +342,10 @@
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -363,10 +357,10 @@
       <c r="A7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="n">
@@ -375,13 +369,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="n">
@@ -393,10 +387,10 @@
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="6" t="n">
@@ -408,10 +402,10 @@
       <c r="A10" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="4" t="n">
         <v>944168</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="7" t="n">
@@ -423,10 +417,10 @@
       <c r="A11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="4" t="n">
         <v>1245501</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="n">
@@ -438,10 +432,10 @@
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="4" t="n">
         <v>944162</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="n">
@@ -453,13 +447,13 @@
       <c r="A13" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="8" t="n">
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -468,13 +462,28 @@
       <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="9" t="n">
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>944181</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -485,10 +494,11 @@
     <hyperlink ref="C12" r:id="rId2" display="kurnool_eGov@123"/>
     <hyperlink ref="C13" r:id="rId3" display="kurnool_eGov@123"/>
     <hyperlink ref="C14" r:id="rId4" display="kurnool_eGov@123"/>
+    <hyperlink ref="C15" r:id="rId5" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-6014] Added advertisement tax collection feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -148,6 +148,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,6 +170,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +264,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -275,18 +277,18 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.5612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.7448979591837"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="17.3061224489796"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,8 +527,8 @@
         <v>5</v>
       </c>
       <c r="D15" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5902] Completed the water collection charges with different mode of payments
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t xml:space="preserve">0944166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.Mohammed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dramachandra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra</t>
   </si>
 </sst>
 </file>
@@ -231,7 +240,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,10 +275,6 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -290,21 +295,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="257" min="27" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +652,52 @@
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>944162</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -666,6 +716,8 @@
     <hyperlink ref="C20" r:id="rId10" display="kurnool_eGov@123"/>
     <hyperlink ref="C21" r:id="rId11" display="kurnool_eGov@123"/>
     <hyperlink ref="C22" r:id="rId12" display="kurnool_eGov@123"/>
+    <hyperlink ref="C23" r:id="rId13" display="kurnool_eGov@123"/>
+    <hyperlink ref="C24" r:id="rId14" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[PHOENIX-6059] updated general revision petition
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -5,177 +5,175 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
-  <si>
-    <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hasZone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juniorAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kurnool_eGov@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billCollector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">946800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0935528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egovernments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assistantEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0954568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seniorAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adm_manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assis_Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountsOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assistantExaminer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0947241</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examiner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0800129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">creator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0942870</t>
-  </si>
-  <si>
-    <t xml:space="preserve">superIntendent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seniorAssistant1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">councilCreator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">councilClerk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sanitaryInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944661</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adm_manager_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mohammed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramachandra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">citizen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9036544535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">akhi2506</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeputyExecutiveEngineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1048833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Executive_engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0905867</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanuman</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+  <si>
+    <t>dataName</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>hasZone</t>
+  </si>
+  <si>
+    <t>juniorAssistant</t>
+  </si>
+  <si>
+    <t>944177</t>
+  </si>
+  <si>
+    <t>kurnool_eGov@123</t>
+  </si>
+  <si>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>0944206</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>944210</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>946800</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>0935528</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>egovernments</t>
+  </si>
+  <si>
+    <t>assistantEngineer</t>
+  </si>
+  <si>
+    <t>0954568</t>
+  </si>
+  <si>
+    <t>seniorAssistant</t>
+  </si>
+  <si>
+    <t>944178</t>
+  </si>
+  <si>
+    <t>adm_manager</t>
+  </si>
+  <si>
+    <t>assis_Engineer</t>
+  </si>
+  <si>
+    <t>accountsOfficer</t>
+  </si>
+  <si>
+    <t>assistantExaminer</t>
+  </si>
+  <si>
+    <t>0947241</t>
+  </si>
+  <si>
+    <t>examiner</t>
+  </si>
+  <si>
+    <t>0800129</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>0944181</t>
+  </si>
+  <si>
+    <t>deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t>0942870</t>
+  </si>
+  <si>
+    <t>superIntendent</t>
+  </si>
+  <si>
+    <t>seniorAssistant1</t>
+  </si>
+  <si>
+    <t>councilCreator</t>
+  </si>
+  <si>
+    <t>0944208</t>
+  </si>
+  <si>
+    <t>councilClerk</t>
+  </si>
+  <si>
+    <t>0944179</t>
+  </si>
+  <si>
+    <t>sanitaryInspector</t>
+  </si>
+  <si>
+    <t>944661</t>
+  </si>
+  <si>
+    <t>adm_manager_1</t>
+  </si>
+  <si>
+    <t>0944166</t>
+  </si>
+  <si>
+    <t>Mohammed</t>
+  </si>
+  <si>
+    <t>Ramachandra</t>
+  </si>
+  <si>
+    <t>S.Ravindra</t>
+  </si>
+  <si>
+    <t>citizen</t>
+  </si>
+  <si>
+    <t>9036544535</t>
+  </si>
+  <si>
+    <t>akhi2506</t>
+  </si>
+  <si>
+    <t>DeputyExecutiveEngineer_1</t>
+  </si>
+  <si>
+    <t>1048833</t>
+  </si>
+  <si>
+    <t>Executive_engineer</t>
+  </si>
+  <si>
+    <t>0905867</t>
+  </si>
+  <si>
+    <t>Hanuman</t>
   </si>
 </sst>
 </file>
@@ -183,12 +181,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -217,12 +215,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -270,7 +262,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,15 +271,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,14 +297,6 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -335,73 +319,74 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.7295918367347"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4948979591837"/>
     <col collapsed="false" hidden="false" max="26" min="5" style="1" width="15.3877551020408"/>
     <col collapsed="false" hidden="false" max="257" min="27" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -413,10 +398,10 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="n">
@@ -428,10 +413,10 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="n">
@@ -443,10 +428,10 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="n">
@@ -458,10 +443,10 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="n">
@@ -470,13 +455,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="6" t="n">
@@ -488,10 +473,10 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="n">
@@ -503,10 +488,10 @@
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="4" t="n">
         <v>944168</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7" t="n">
@@ -518,10 +503,10 @@
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="4" t="n">
         <v>1245501</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="6" t="n">
@@ -533,10 +518,10 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="4" t="n">
         <v>944162</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="6" t="n">
@@ -548,10 +533,10 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="n">
@@ -563,10 +548,10 @@
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="n">
@@ -578,8 +563,8 @@
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -591,10 +576,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -606,7 +591,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>944162</v>
@@ -620,10 +605,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2" t="n">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="n">
         <v>944176</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -636,12 +621,12 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="1" t="n">
@@ -651,12 +636,12 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="n">
@@ -666,12 +651,12 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="n">
@@ -681,10 +666,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -696,12 +681,12 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="B23" s="4" t="n">
         <v>944162</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="6" t="n">
@@ -711,12 +696,12 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="n">
@@ -726,12 +711,12 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1" t="n">
@@ -741,13 +726,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>46</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D26" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -756,11 +741,11 @@
     </row>
     <row r="27" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B27" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
@@ -770,11 +755,11 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="A28" s="2" t="s">
         <v>50</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -786,15 +771,15 @@
     </row>
     <row r="29" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="10" t="n">
+      <c r="D29" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -821,7 +806,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-6061] changes in Grievances
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/loginTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>dataName</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>0956637</t>
+  </si>
+  <si>
+    <t>CSCUser</t>
+  </si>
+  <si>
+    <t>CSCUSER</t>
+  </si>
+  <si>
+    <t>PublicHealthJA</t>
+  </si>
+  <si>
+    <t>0944182</t>
   </si>
 </sst>
 </file>
@@ -545,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW30"/>
+  <dimension ref="A1:IW32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E31:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1037,35 @@
       <c r="D30" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1047,8 +1088,9 @@
     <hyperlink ref="C28" r:id="rId16"/>
     <hyperlink ref="C29" r:id="rId17"/>
     <hyperlink ref="C30" r:id="rId18"/>
+    <hyperlink ref="C31" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>